<commit_message>
improved summary extraction function with improved consensus calculation and reran whole script
</commit_message>
<xml_diff>
--- a/data/processed_data/voted_laws_migration.xlsx
+++ b/data/processed_data/voted_laws_migration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e8b233dcb308e1e/Dokumente/_Masterstudium/Thesis/Thesis_db/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e8b233dcb308e1e/Dokumente/_Masterstudium/Thesis/Thesis_db/data/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="47" documentId="8_{0FD23916-4D40-4BAF-BE90-2C0AFE70B237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ED80BF4-FC5C-413F-89CE-40E3B4FF1389}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1ED53B26-0918-43D7-A511-99BD0BF912A4}"/>
+    <workbookView minimized="1" xWindow="2280" yWindow="2280" windowWidth="5770" windowHeight="7270" xr2:uid="{1ED53B26-0918-43D7-A511-99BD0BF912A4}"/>
   </bookViews>
   <sheets>
     <sheet name="voted_laws_migration" sheetId="1" r:id="rId1"/>
@@ -2739,8 +2739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEDA577-CCB7-4000-9CAF-F6213670DC84}">
   <dimension ref="A1:BB66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J57" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="AU39" sqref="AU39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>